<commit_message>
Frame in main application with self definition
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRussell\PycharmProjects\Lesson1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRussell\PycharmProjects\SHED_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5408656E-0B3C-4DD1-9B12-76C56347873D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB73EF4A-161A-44A8-840C-70F9B936EA00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="0" windowWidth="10656" windowHeight="9000" xr2:uid="{82A4BAAA-6ED8-4E76-AA6A-33CFEDDEFD2A}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="2" xr2:uid="{82A4BAAA-6ED8-4E76-AA6A-33CFEDDEFD2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Startup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="70">
   <si>
     <t>SHED Auxiliary systems config file</t>
   </si>
@@ -220,6 +222,30 @@
   </si>
   <si>
     <t>// Valve voltage which corresponding pump turns off to protect against deadheading</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>v6</t>
+  </si>
+  <si>
+    <t>v7</t>
+  </si>
+  <si>
+    <t>v8</t>
   </si>
 </sst>
 </file>
@@ -583,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7068524D-5CCD-4349-A0BD-476FA9D60713}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -870,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C548B4C-BA48-40B5-B431-A1AA20E76153}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1314,4 +1340,147 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B2DD31-8BBF-4700-B5F4-2489BD8E6472}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>